<commit_message>
Cambios post reunión con Gregorio, conclusiones incluidas en el log
</commit_message>
<xml_diff>
--- a/data/TOPICS.xlsx
+++ b/data/TOPICS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univmurcia-my.sharepoint.com/personal/gbernabe_um_es/Documents/2024-2025/eventos/enero/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Musatom\Documents\Universidad\Master\TFM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{58D7D497-A748-4561-BD72-053223F4F009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D58813FB-C153-4D7F-B243-2EDB466B5DF0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18225CA2-D1F7-4A8C-A2A2-C106F4B82FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CÓDIGOS" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="423">
   <si>
     <t>VAR</t>
   </si>
@@ -2896,6 +2896,27 @@
   </si>
   <si>
     <t>Buenos ejemplos sobre los últimos cambios en las reglas del juego. Normalmente irá acompañando a otros códigos.</t>
+  </si>
+  <si>
+    <t>CONTROL DISCIPLINARIO</t>
+  </si>
+  <si>
+    <t>CONTROL DE PARTIDO</t>
+  </si>
+  <si>
+    <t>CONDICION TECNICA / INCIDENTES DE AREA</t>
+  </si>
+  <si>
+    <t>ASISTENTES</t>
+  </si>
+  <si>
+    <t>JUGADAS DE AREA</t>
+  </si>
+  <si>
+    <t>CONDICION FISICA</t>
+  </si>
+  <si>
+    <t>TRABAJO EN EQUIPO</t>
   </si>
 </sst>
 </file>
@@ -3697,11 +3718,22 @@
     <xf numFmtId="49" fontId="8" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3711,24 +3743,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4009,8 +4030,8 @@
   </sheetPr>
   <dimension ref="A1:Y166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4054,7 +4075,7 @@
     </row>
     <row r="2" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="79" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="80"/>
@@ -4127,7 +4148,9 @@
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>416</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -4158,7 +4181,7 @@
       <c r="D5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="6"/>
@@ -4193,7 +4216,7 @@
       <c r="D6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="89"/>
+      <c r="E6" s="83"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -4226,7 +4249,7 @@
       <c r="D7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="89"/>
+      <c r="E7" s="83"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4259,7 +4282,7 @@
       <c r="D8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="89"/>
+      <c r="E8" s="83"/>
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -4292,7 +4315,7 @@
       <c r="D9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="89"/>
+      <c r="E9" s="83"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -4325,7 +4348,7 @@
       <c r="D10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="89"/>
+      <c r="E10" s="83"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -4358,7 +4381,7 @@
       <c r="D11" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="89"/>
+      <c r="E11" s="83"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -4391,7 +4414,7 @@
       <c r="D12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="89"/>
+      <c r="E12" s="83"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -4424,7 +4447,7 @@
       <c r="D13" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="89"/>
+      <c r="E13" s="83"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -4457,7 +4480,7 @@
       <c r="D14" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="89"/>
+      <c r="E14" s="83"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -4490,7 +4513,7 @@
       <c r="D15" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="89"/>
+      <c r="E15" s="83"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -4523,7 +4546,7 @@
       <c r="D16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="89"/>
+      <c r="E16" s="83"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -4556,7 +4579,7 @@
       <c r="D17" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="89"/>
+      <c r="E17" s="83"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -4589,7 +4612,7 @@
       <c r="D18" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="89"/>
+      <c r="E18" s="83"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -4622,7 +4645,7 @@
       <c r="D19" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="89"/>
+      <c r="E19" s="83"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -4655,7 +4678,7 @@
       <c r="D20" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="89"/>
+      <c r="E20" s="83"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -4688,7 +4711,7 @@
       <c r="D21" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="89"/>
+      <c r="E21" s="83"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -4721,7 +4744,7 @@
       <c r="D22" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="89"/>
+      <c r="E22" s="83"/>
       <c r="F22" s="6"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -4754,7 +4777,7 @@
       <c r="D23" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="89"/>
+      <c r="E23" s="83"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -4787,7 +4810,7 @@
       <c r="D24" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="90"/>
+      <c r="E24" s="84"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -4811,7 +4834,7 @@
     </row>
     <row r="25" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="87"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="80"/>
       <c r="D25" s="80"/>
       <c r="E25" s="81"/>
@@ -4847,7 +4870,9 @@
       <c r="D26" s="14"/>
       <c r="E26" s="15"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>417</v>
+      </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -4878,7 +4903,7 @@
       <c r="D27" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="88" t="s">
         <v>78</v>
       </c>
       <c r="F27" s="6"/>
@@ -4913,7 +4938,7 @@
       <c r="D28" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="84"/>
+      <c r="E28" s="89"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -4946,7 +4971,7 @@
       <c r="D29" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="84"/>
+      <c r="E29" s="89"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -4979,7 +5004,7 @@
       <c r="D30" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="84"/>
+      <c r="E30" s="89"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -5012,7 +5037,7 @@
       <c r="D31" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="84"/>
+      <c r="E31" s="89"/>
       <c r="F31" s="6"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -5045,7 +5070,7 @@
       <c r="D32" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E32" s="84"/>
+      <c r="E32" s="89"/>
       <c r="F32" s="6"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -5076,7 +5101,7 @@
       <c r="D33" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E33" s="84"/>
+      <c r="E33" s="89"/>
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -5109,7 +5134,7 @@
       <c r="D34" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="84"/>
+      <c r="E34" s="89"/>
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -5142,7 +5167,7 @@
       <c r="D35" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="84"/>
+      <c r="E35" s="89"/>
       <c r="F35" s="6"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
@@ -5175,7 +5200,7 @@
       <c r="D36" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="84"/>
+      <c r="E36" s="89"/>
       <c r="F36" s="6"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
@@ -5208,7 +5233,7 @@
       <c r="D37" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="84"/>
+      <c r="E37" s="89"/>
       <c r="F37" s="6"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -5241,7 +5266,7 @@
       <c r="D38" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="84"/>
+      <c r="E38" s="89"/>
       <c r="F38" s="6"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -5274,7 +5299,7 @@
       <c r="D39" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="E39" s="84"/>
+      <c r="E39" s="89"/>
       <c r="F39" s="6"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -5307,7 +5332,7 @@
       <c r="D40" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="E40" s="84"/>
+      <c r="E40" s="89"/>
       <c r="F40" s="6"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -5340,7 +5365,7 @@
       <c r="D41" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="84"/>
+      <c r="E41" s="89"/>
       <c r="F41" s="6"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -5373,7 +5398,7 @@
       <c r="D42" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="E42" s="84"/>
+      <c r="E42" s="89"/>
       <c r="F42" s="6"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
@@ -5406,7 +5431,7 @@
       <c r="D43" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E43" s="84"/>
+      <c r="E43" s="89"/>
       <c r="F43" s="6"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -5439,7 +5464,7 @@
       <c r="D44" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="E44" s="84"/>
+      <c r="E44" s="89"/>
       <c r="F44" s="6"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
@@ -5472,7 +5497,7 @@
       <c r="D45" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="84"/>
+      <c r="E45" s="89"/>
       <c r="F45" s="6"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
@@ -5505,7 +5530,7 @@
       <c r="D46" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="84"/>
+      <c r="E46" s="89"/>
       <c r="F46" s="6"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
@@ -5538,7 +5563,7 @@
       <c r="D47" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="84"/>
+      <c r="E47" s="89"/>
       <c r="F47" s="6"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -5571,7 +5596,7 @@
       <c r="D48" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="84"/>
+      <c r="E48" s="89"/>
       <c r="F48" s="6"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -5604,7 +5629,7 @@
       <c r="D49" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E49" s="84"/>
+      <c r="E49" s="89"/>
       <c r="F49" s="6"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -5637,7 +5662,7 @@
       <c r="D50" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="E50" s="84"/>
+      <c r="E50" s="89"/>
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -5670,7 +5695,7 @@
       <c r="D51" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E51" s="84"/>
+      <c r="E51" s="89"/>
       <c r="F51" s="6"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -5703,7 +5728,7 @@
       <c r="D52" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="E52" s="84"/>
+      <c r="E52" s="89"/>
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
@@ -5736,7 +5761,7 @@
       <c r="D53" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="E53" s="84"/>
+      <c r="E53" s="89"/>
       <c r="F53" s="6"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
@@ -5769,7 +5794,7 @@
       <c r="D54" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="E54" s="84"/>
+      <c r="E54" s="89"/>
       <c r="F54" s="6"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -5802,7 +5827,7 @@
       <c r="D55" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="E55" s="84"/>
+      <c r="E55" s="89"/>
       <c r="F55" s="6"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -5835,7 +5860,7 @@
       <c r="D56" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="E56" s="84"/>
+      <c r="E56" s="89"/>
       <c r="F56" s="6"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
@@ -5868,7 +5893,7 @@
       <c r="D57" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="E57" s="84"/>
+      <c r="E57" s="89"/>
       <c r="F57" s="6"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -5901,7 +5926,7 @@
       <c r="D58" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="E58" s="84"/>
+      <c r="E58" s="89"/>
       <c r="F58" s="6"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
@@ -5934,7 +5959,7 @@
       <c r="D59" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="E59" s="85"/>
+      <c r="E59" s="90"/>
       <c r="F59" s="6"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -5958,7 +5983,7 @@
     </row>
     <row r="60" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="87"/>
+      <c r="B60" s="85"/>
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="81"/>
@@ -5998,7 +6023,9 @@
         <v>173</v>
       </c>
       <c r="F61" s="6"/>
-      <c r="G61" s="7"/>
+      <c r="G61" s="7" t="s">
+        <v>418</v>
+      </c>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -6029,7 +6056,7 @@
       <c r="D62" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E62" s="83"/>
+      <c r="E62" s="88"/>
       <c r="F62" s="6"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
@@ -6062,7 +6089,7 @@
       <c r="D63" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="E63" s="84"/>
+      <c r="E63" s="89"/>
       <c r="F63" s="6"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
@@ -6095,7 +6122,7 @@
       <c r="D64" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="E64" s="84"/>
+      <c r="E64" s="89"/>
       <c r="F64" s="6"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
@@ -6128,7 +6155,7 @@
       <c r="D65" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="E65" s="84"/>
+      <c r="E65" s="89"/>
       <c r="F65" s="6"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
@@ -6161,7 +6188,7 @@
       <c r="D66" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="E66" s="84"/>
+      <c r="E66" s="89"/>
       <c r="F66" s="6"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
@@ -6194,7 +6221,7 @@
       <c r="D67" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="E67" s="84"/>
+      <c r="E67" s="89"/>
       <c r="F67" s="6"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
@@ -6227,7 +6254,7 @@
       <c r="D68" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="E68" s="84"/>
+      <c r="E68" s="89"/>
       <c r="F68" s="6"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
@@ -6260,7 +6287,7 @@
       <c r="D69" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="E69" s="86"/>
+      <c r="E69" s="91"/>
       <c r="F69" s="6"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
@@ -6284,7 +6311,7 @@
     </row>
     <row r="70" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
-      <c r="B70" s="87"/>
+      <c r="B70" s="85"/>
       <c r="C70" s="80"/>
       <c r="D70" s="80"/>
       <c r="E70" s="81"/>
@@ -6353,7 +6380,7 @@
       <c r="D72" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="E72" s="88" t="s">
+      <c r="E72" s="92" t="s">
         <v>204</v>
       </c>
       <c r="F72" s="6"/>
@@ -6388,7 +6415,7 @@
       <c r="D73" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="E73" s="89"/>
+      <c r="E73" s="83"/>
       <c r="F73" s="6"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
@@ -6421,7 +6448,7 @@
       <c r="D74" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="E74" s="89"/>
+      <c r="E74" s="83"/>
       <c r="F74" s="6"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
@@ -6454,7 +6481,7 @@
       <c r="D75" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="E75" s="89"/>
+      <c r="E75" s="83"/>
       <c r="F75" s="6"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
@@ -6487,7 +6514,7 @@
       <c r="D76" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="E76" s="89"/>
+      <c r="E76" s="83"/>
       <c r="F76" s="6"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
@@ -6520,7 +6547,7 @@
       <c r="D77" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="E77" s="89"/>
+      <c r="E77" s="83"/>
       <c r="F77" s="6"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
@@ -6553,7 +6580,7 @@
       <c r="D78" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="E78" s="89"/>
+      <c r="E78" s="83"/>
       <c r="F78" s="6"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
@@ -6586,7 +6613,7 @@
       <c r="D79" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="E79" s="90"/>
+      <c r="E79" s="84"/>
       <c r="F79" s="6"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
@@ -6610,7 +6637,7 @@
     </row>
     <row r="80" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="B80" s="87"/>
+      <c r="B80" s="85"/>
       <c r="C80" s="80"/>
       <c r="D80" s="80"/>
       <c r="E80" s="81"/>
@@ -6646,7 +6673,9 @@
       <c r="D81" s="14"/>
       <c r="E81" s="15"/>
       <c r="F81" s="6"/>
-      <c r="G81" s="7"/>
+      <c r="G81" s="7" t="s">
+        <v>419</v>
+      </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
@@ -6677,7 +6706,7 @@
       <c r="D82" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="E82" s="88" t="s">
+      <c r="E82" s="92" t="s">
         <v>224</v>
       </c>
       <c r="F82" s="6"/>
@@ -6712,7 +6741,7 @@
       <c r="D83" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="E83" s="89"/>
+      <c r="E83" s="83"/>
       <c r="F83" s="6"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
@@ -6745,7 +6774,7 @@
       <c r="D84" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="E84" s="89"/>
+      <c r="E84" s="83"/>
       <c r="F84" s="6"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
@@ -6778,7 +6807,7 @@
       <c r="D85" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="E85" s="89"/>
+      <c r="E85" s="83"/>
       <c r="F85" s="6"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
@@ -6811,7 +6840,7 @@
       <c r="D86" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="E86" s="89"/>
+      <c r="E86" s="83"/>
       <c r="F86" s="6"/>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
@@ -6844,7 +6873,7 @@
       <c r="D87" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="E87" s="89"/>
+      <c r="E87" s="83"/>
       <c r="F87" s="6"/>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
@@ -6877,7 +6906,7 @@
       <c r="D88" s="54" t="s">
         <v>239</v>
       </c>
-      <c r="E88" s="89"/>
+      <c r="E88" s="83"/>
       <c r="F88" s="6"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
@@ -6910,7 +6939,7 @@
       <c r="D89" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="E89" s="89"/>
+      <c r="E89" s="83"/>
       <c r="F89" s="6"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
@@ -6943,7 +6972,7 @@
       <c r="D90" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="E90" s="89"/>
+      <c r="E90" s="83"/>
       <c r="F90" s="6"/>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
@@ -6976,7 +7005,7 @@
       <c r="D91" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="E91" s="89"/>
+      <c r="E91" s="83"/>
       <c r="F91" s="6"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
@@ -7009,7 +7038,7 @@
       <c r="D92" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="E92" s="89"/>
+      <c r="E92" s="83"/>
       <c r="F92" s="6"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
@@ -7042,7 +7071,7 @@
       <c r="D93" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="E93" s="89"/>
+      <c r="E93" s="83"/>
       <c r="F93" s="6"/>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
@@ -7075,7 +7104,7 @@
       <c r="D94" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="E94" s="90"/>
+      <c r="E94" s="84"/>
       <c r="F94" s="6"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
@@ -7099,7 +7128,7 @@
     </row>
     <row r="95" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
-      <c r="B95" s="87"/>
+      <c r="B95" s="85"/>
       <c r="C95" s="80"/>
       <c r="D95" s="80"/>
       <c r="E95" s="81"/>
@@ -7135,7 +7164,9 @@
       <c r="D96" s="14"/>
       <c r="E96" s="15"/>
       <c r="F96" s="6"/>
-      <c r="G96" s="7"/>
+      <c r="G96" s="7" t="s">
+        <v>420</v>
+      </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
@@ -7166,7 +7197,7 @@
       <c r="D97" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="E97" s="91" t="s">
+      <c r="E97" s="93" t="s">
         <v>259</v>
       </c>
       <c r="F97" s="6"/>
@@ -7201,7 +7232,7 @@
       <c r="D98" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="E98" s="89"/>
+      <c r="E98" s="83"/>
       <c r="F98" s="6"/>
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
@@ -7234,7 +7265,7 @@
       <c r="D99" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="E99" s="89"/>
+      <c r="E99" s="83"/>
       <c r="F99" s="6"/>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
@@ -7267,7 +7298,7 @@
       <c r="D100" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="E100" s="89"/>
+      <c r="E100" s="83"/>
       <c r="F100" s="6"/>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
@@ -7300,7 +7331,7 @@
       <c r="D101" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="E101" s="89"/>
+      <c r="E101" s="83"/>
       <c r="F101" s="6"/>
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
@@ -7333,7 +7364,7 @@
       <c r="D102" s="67" t="s">
         <v>271</v>
       </c>
-      <c r="E102" s="89"/>
+      <c r="E102" s="83"/>
       <c r="F102" s="6"/>
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
@@ -7366,7 +7397,7 @@
       <c r="D103" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="E103" s="89"/>
+      <c r="E103" s="83"/>
       <c r="F103" s="6"/>
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
@@ -7399,7 +7430,7 @@
       <c r="D104" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="E104" s="89"/>
+      <c r="E104" s="83"/>
       <c r="F104" s="6"/>
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
@@ -7432,7 +7463,7 @@
       <c r="D105" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="E105" s="89"/>
+      <c r="E105" s="83"/>
       <c r="F105" s="6"/>
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
@@ -7465,7 +7496,7 @@
       <c r="D106" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="E106" s="89"/>
+      <c r="E106" s="83"/>
       <c r="F106" s="6"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
@@ -7498,7 +7529,7 @@
       <c r="D107" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="E107" s="89"/>
+      <c r="E107" s="83"/>
       <c r="F107" s="6"/>
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
@@ -7531,7 +7562,7 @@
       <c r="D108" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="E108" s="89"/>
+      <c r="E108" s="83"/>
       <c r="F108" s="6"/>
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
@@ -7564,7 +7595,7 @@
       <c r="D109" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="E109" s="89"/>
+      <c r="E109" s="83"/>
       <c r="F109" s="6"/>
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
@@ -7597,7 +7628,7 @@
       <c r="D110" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="E110" s="89"/>
+      <c r="E110" s="83"/>
       <c r="F110" s="6"/>
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
@@ -7630,7 +7661,7 @@
       <c r="D111" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="E111" s="89"/>
+      <c r="E111" s="83"/>
       <c r="F111" s="6"/>
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
@@ -7663,7 +7694,7 @@
       <c r="D112" s="30" t="s">
         <v>297</v>
       </c>
-      <c r="E112" s="89"/>
+      <c r="E112" s="83"/>
       <c r="F112" s="6"/>
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
@@ -7696,7 +7727,7 @@
       <c r="D113" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="E113" s="89"/>
+      <c r="E113" s="83"/>
       <c r="F113" s="6"/>
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
@@ -7729,7 +7760,7 @@
       <c r="D114" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="E114" s="92"/>
+      <c r="E114" s="94"/>
       <c r="F114" s="6"/>
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
@@ -7753,7 +7784,7 @@
     </row>
     <row r="115" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
-      <c r="B115" s="87"/>
+      <c r="B115" s="85"/>
       <c r="C115" s="80"/>
       <c r="D115" s="80"/>
       <c r="E115" s="81"/>
@@ -7789,7 +7820,9 @@
       <c r="D116" s="14"/>
       <c r="E116" s="15"/>
       <c r="F116" s="6"/>
-      <c r="G116" s="7"/>
+      <c r="G116" s="7" t="s">
+        <v>421</v>
+      </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
@@ -7820,7 +7853,7 @@
       <c r="D117" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="E117" s="88" t="s">
+      <c r="E117" s="92" t="s">
         <v>306</v>
       </c>
       <c r="F117" s="6"/>
@@ -7855,7 +7888,7 @@
       <c r="D118" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="E118" s="89"/>
+      <c r="E118" s="83"/>
       <c r="F118" s="6"/>
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
@@ -7888,7 +7921,7 @@
       <c r="D119" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="E119" s="89"/>
+      <c r="E119" s="83"/>
       <c r="F119" s="6"/>
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
@@ -7921,7 +7954,7 @@
       <c r="D120" s="50" t="s">
         <v>314</v>
       </c>
-      <c r="E120" s="89"/>
+      <c r="E120" s="83"/>
       <c r="F120" s="6"/>
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
@@ -7954,7 +7987,7 @@
       <c r="D121" s="70" t="s">
         <v>317</v>
       </c>
-      <c r="E121" s="89"/>
+      <c r="E121" s="83"/>
       <c r="F121" s="6"/>
       <c r="G121" s="7"/>
       <c r="H121" s="7"/>
@@ -7987,7 +8020,7 @@
       <c r="D122" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="E122" s="89"/>
+      <c r="E122" s="83"/>
       <c r="F122" s="6"/>
       <c r="G122" s="7"/>
       <c r="H122" s="7"/>
@@ -8020,7 +8053,7 @@
       <c r="D123" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="E123" s="89"/>
+      <c r="E123" s="83"/>
       <c r="F123" s="6"/>
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
@@ -8053,7 +8086,7 @@
       <c r="D124" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="E124" s="89"/>
+      <c r="E124" s="83"/>
       <c r="F124" s="6"/>
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
@@ -8086,7 +8119,7 @@
       <c r="D125" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="E125" s="89"/>
+      <c r="E125" s="83"/>
       <c r="F125" s="6"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
@@ -8119,7 +8152,7 @@
       <c r="D126" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="E126" s="89"/>
+      <c r="E126" s="83"/>
       <c r="F126" s="6"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
@@ -8152,7 +8185,7 @@
       <c r="D127" s="30" t="s">
         <v>335</v>
       </c>
-      <c r="E127" s="89"/>
+      <c r="E127" s="83"/>
       <c r="F127" s="6"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
@@ -8185,7 +8218,7 @@
       <c r="D128" s="33" t="s">
         <v>338</v>
       </c>
-      <c r="E128" s="89"/>
+      <c r="E128" s="83"/>
       <c r="F128" s="6"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
@@ -8218,7 +8251,7 @@
       <c r="D129" s="33" t="s">
         <v>341</v>
       </c>
-      <c r="E129" s="89"/>
+      <c r="E129" s="83"/>
       <c r="F129" s="6"/>
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
@@ -8251,7 +8284,7 @@
       <c r="D130" s="24" t="s">
         <v>344</v>
       </c>
-      <c r="E130" s="89"/>
+      <c r="E130" s="83"/>
       <c r="F130" s="6"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
@@ -8284,7 +8317,7 @@
       <c r="D131" s="52" t="s">
         <v>347</v>
       </c>
-      <c r="E131" s="89"/>
+      <c r="E131" s="83"/>
       <c r="F131" s="6"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
@@ -8317,7 +8350,7 @@
       <c r="D132" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="E132" s="92"/>
+      <c r="E132" s="94"/>
       <c r="F132" s="6"/>
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
@@ -8341,7 +8374,7 @@
     </row>
     <row r="133" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
-      <c r="B133" s="87"/>
+      <c r="B133" s="85"/>
       <c r="C133" s="80"/>
       <c r="D133" s="80"/>
       <c r="E133" s="81"/>
@@ -8377,7 +8410,9 @@
       <c r="D134" s="14"/>
       <c r="E134" s="15"/>
       <c r="F134" s="6"/>
-      <c r="G134" s="7"/>
+      <c r="G134" s="7" t="s">
+        <v>416</v>
+      </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
@@ -8408,7 +8443,7 @@
       <c r="D135" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="E135" s="88" t="s">
+      <c r="E135" s="92" t="s">
         <v>353</v>
       </c>
       <c r="F135" s="6"/>
@@ -8443,7 +8478,7 @@
       <c r="D136" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="E136" s="89"/>
+      <c r="E136" s="83"/>
       <c r="F136" s="6"/>
       <c r="G136" s="7"/>
       <c r="H136" s="7"/>
@@ -8476,7 +8511,7 @@
       <c r="D137" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="E137" s="89"/>
+      <c r="E137" s="83"/>
       <c r="F137" s="6"/>
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
@@ -8509,7 +8544,7 @@
       <c r="D138" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="E138" s="89"/>
+      <c r="E138" s="83"/>
       <c r="F138" s="6"/>
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
@@ -8542,7 +8577,7 @@
       <c r="D139" s="24" t="s">
         <v>363</v>
       </c>
-      <c r="E139" s="89"/>
+      <c r="E139" s="83"/>
       <c r="F139" s="6"/>
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
@@ -8575,7 +8610,7 @@
       <c r="D140" s="38" t="s">
         <v>365</v>
       </c>
-      <c r="E140" s="89"/>
+      <c r="E140" s="83"/>
       <c r="F140" s="6"/>
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
@@ -8608,7 +8643,7 @@
       <c r="D141" s="36" t="s">
         <v>367</v>
       </c>
-      <c r="E141" s="92"/>
+      <c r="E141" s="94"/>
       <c r="F141" s="6"/>
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
@@ -8632,7 +8667,7 @@
     </row>
     <row r="142" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
-      <c r="B142" s="87"/>
+      <c r="B142" s="85"/>
       <c r="C142" s="80"/>
       <c r="D142" s="80"/>
       <c r="E142" s="81"/>
@@ -8672,7 +8707,9 @@
         <v>370</v>
       </c>
       <c r="F143" s="6"/>
-      <c r="G143" s="7"/>
+      <c r="G143" s="7" t="s">
+        <v>422</v>
+      </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
@@ -8694,7 +8731,7 @@
     </row>
     <row r="144" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
-      <c r="B144" s="87"/>
+      <c r="B144" s="85"/>
       <c r="C144" s="80"/>
       <c r="D144" s="80"/>
       <c r="E144" s="81"/>
@@ -8763,7 +8800,7 @@
       <c r="D146" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="E146" s="88" t="s">
+      <c r="E146" s="92" t="s">
         <v>374</v>
       </c>
       <c r="F146" s="6"/>
@@ -8798,7 +8835,7 @@
       <c r="D147" s="52" t="s">
         <v>376</v>
       </c>
-      <c r="E147" s="89"/>
+      <c r="E147" s="83"/>
       <c r="F147" s="6"/>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
@@ -8831,7 +8868,7 @@
       <c r="D148" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="E148" s="89"/>
+      <c r="E148" s="83"/>
       <c r="F148" s="6"/>
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
@@ -8864,7 +8901,7 @@
       <c r="D149" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="E149" s="89"/>
+      <c r="E149" s="83"/>
       <c r="F149" s="6"/>
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
@@ -8897,7 +8934,7 @@
       <c r="D150" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E150" s="89"/>
+      <c r="E150" s="83"/>
       <c r="F150" s="6"/>
       <c r="G150" s="7"/>
       <c r="H150" s="7"/>
@@ -8930,7 +8967,7 @@
       <c r="D151" s="36" t="s">
         <v>388</v>
       </c>
-      <c r="E151" s="89"/>
+      <c r="E151" s="83"/>
       <c r="F151" s="6"/>
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
@@ -8963,7 +9000,7 @@
       <c r="D152" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="E152" s="89"/>
+      <c r="E152" s="83"/>
       <c r="F152" s="6"/>
       <c r="G152" s="7"/>
       <c r="H152" s="7"/>
@@ -8996,7 +9033,7 @@
       <c r="D153" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="E153" s="90"/>
+      <c r="E153" s="84"/>
       <c r="F153" s="6"/>
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
@@ -9020,7 +9057,7 @@
     </row>
     <row r="154" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
-      <c r="B154" s="87"/>
+      <c r="B154" s="85"/>
       <c r="C154" s="80"/>
       <c r="D154" s="80"/>
       <c r="E154" s="81"/>
@@ -9047,7 +9084,7 @@
     </row>
     <row r="155" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
-      <c r="B155" s="79"/>
+      <c r="B155" s="86"/>
       <c r="C155" s="80"/>
       <c r="D155" s="80"/>
       <c r="E155" s="81"/>
@@ -9109,7 +9146,7 @@
     </row>
     <row r="157" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
-      <c r="B157" s="79"/>
+      <c r="B157" s="86"/>
       <c r="C157" s="80"/>
       <c r="D157" s="80"/>
       <c r="E157" s="81"/>
@@ -9171,7 +9208,7 @@
     </row>
     <row r="159" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
-      <c r="B159" s="79"/>
+      <c r="B159" s="86"/>
       <c r="C159" s="80"/>
       <c r="D159" s="80"/>
       <c r="E159" s="81"/>
@@ -9233,7 +9270,7 @@
     </row>
     <row r="161" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
-      <c r="B161" s="79"/>
+      <c r="B161" s="86"/>
       <c r="C161" s="80"/>
       <c r="D161" s="80"/>
       <c r="E161" s="81"/>
@@ -9295,7 +9332,7 @@
     </row>
     <row r="163" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
-      <c r="B163" s="79"/>
+      <c r="B163" s="86"/>
       <c r="C163" s="80"/>
       <c r="D163" s="80"/>
       <c r="E163" s="81"/>
@@ -9357,7 +9394,7 @@
     </row>
     <row r="165" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
-      <c r="B165" s="82" t="s">
+      <c r="B165" s="87" t="s">
         <v>411</v>
       </c>
       <c r="C165" s="80"/>
@@ -9421,16 +9458,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="E5:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="B155:E155"/>
-    <mergeCell ref="B157:E157"/>
-    <mergeCell ref="B115:E115"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B154:E154"/>
     <mergeCell ref="B159:E159"/>
     <mergeCell ref="B161:E161"/>
     <mergeCell ref="B165:E165"/>
@@ -9447,6 +9474,16 @@
     <mergeCell ref="E135:E141"/>
     <mergeCell ref="B142:E142"/>
     <mergeCell ref="B144:E144"/>
+    <mergeCell ref="B155:E155"/>
+    <mergeCell ref="B157:E157"/>
+    <mergeCell ref="B115:E115"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B154:E154"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E5:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B95:E95"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>